<commit_message>
feat(syncing): Remove empty columns.
</commit_message>
<xml_diff>
--- a/test/files/data_H.xlsx
+++ b/test/files/data_H.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/syncing/test/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0D82AF-065A-9543-B7D7-FF240153EF03}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974CED1C-9F42-C44D-AADC-F9376CAFAE61}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11760" yWindow="460" windowWidth="17040" windowHeight="15220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>x</t>
   </si>
@@ -418,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,8 +436,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -447,8 +450,11 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>0</v>
       </c>
@@ -459,7 +465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -470,7 +476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -481,7 +487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -492,7 +498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -503,7 +509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -514,7 +520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -525,7 +531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -536,7 +542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -547,7 +553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -558,7 +564,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -569,7 +575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -580,7 +586,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -591,7 +597,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>

</xml_diff>